<commit_message>
codes updated to add more data
</commit_message>
<xml_diff>
--- a/data/[R] [Ethnologue] Language diversity index.xlsx
+++ b/data/[R] [Ethnologue] Language diversity index.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14370"/>
+    <workbookView xWindow="480" yWindow="165" windowWidth="27795" windowHeight="14310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,21 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="236">
   <si>
-    <t>Cover- age</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Per- cent</t>
-  </si>
-  <si>
-    <t>Indige- nous</t>
-  </si>
-  <si>
-    <t>Immi- grant</t>
-  </si>
-  <si>
     <t>Count</t>
   </si>
   <si>
@@ -722,6 +707,21 @@
   </si>
   <si>
     <t>Language Diversity Index</t>
+  </si>
+  <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>Total Living Language</t>
+  </si>
+  <si>
+    <t>Percent living language</t>
+  </si>
+  <si>
+    <t>Indigenous living language</t>
+  </si>
+  <si>
+    <t>Immigrant living language</t>
   </si>
 </sst>
 </file>
@@ -1094,13 +1094,13 @@
   <dimension ref="A1:L226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
@@ -1113,34 +1113,34 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" t="s">
         <v>234</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>235</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
       </c>
       <c r="L1">
         <v>2013</v>
@@ -1148,7 +1148,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>0.98799999999999999</v>
@@ -1166,7 +1166,7 @@
         <v>836</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H2" s="4">
         <v>4123564</v>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>0.97299999999999998</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>0.97199999999999998</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>0.96799999999999997</v>
@@ -1262,7 +1262,7 @@
         <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H5" s="4">
         <v>380323</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>0.95899999999999996</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>0.94799999999999995</v>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>0.94499999999999995</v>
@@ -1372,7 +1372,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>0.93200000000000005</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>0.92900000000000005</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>0.92800000000000005</v>
@@ -1468,7 +1468,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>0.92700000000000005</v>
@@ -1486,7 +1486,7 @@
         <v>68</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H12" s="4">
         <v>4370650</v>
@@ -1500,7 +1500,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>0.92200000000000004</v>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>0.91700000000000004</v>
@@ -1564,7 +1564,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
         <v>0.91600000000000004</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B16" s="1">
         <v>0.89900000000000002</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5">
         <v>0.89700000000000002</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B18" s="5">
         <v>0.89100000000000001</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B19" s="5">
         <v>0.878</v>
@@ -1710,7 +1710,7 @@
         <v>75</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H19" s="8">
         <v>3447652</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B20" s="5">
         <v>0.878</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B21" s="5">
         <v>0.874</v>
@@ -1788,7 +1788,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B22" s="5">
         <v>0.86399999999999999</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B23" s="5">
         <v>0.85499999999999998</v>
@@ -1852,7 +1852,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B24" s="5">
         <v>0.85499999999999998</v>
@@ -1884,7 +1884,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B25" s="5">
         <v>0.85399999999999998</v>
@@ -1916,7 +1916,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B26" s="5">
         <v>0.84899999999999998</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B27" s="5">
         <v>0.84499999999999997</v>
@@ -1980,7 +1980,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B28" s="5">
         <v>0.84499999999999997</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5">
         <v>0.83499999999999996</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B30" s="5">
         <v>0.83399999999999996</v>
@@ -2076,7 +2076,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B31" s="5">
         <v>0.81699999999999995</v>
@@ -2094,7 +2094,7 @@
         <v>19</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H31" s="8">
         <v>1033506</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B32" s="5">
         <v>0.81599999999999995</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B33" s="5">
         <v>0.81499999999999995</v>
@@ -2172,7 +2172,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B34" s="5">
         <v>0.79</v>
@@ -2204,7 +2204,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B35" s="5">
         <v>0.78800000000000003</v>
@@ -2236,7 +2236,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B36" s="5">
         <v>0.78300000000000003</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B37" s="5">
         <v>0.78100000000000003</v>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B38" s="5">
         <v>0.78</v>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B39" s="5">
         <v>0.77800000000000002</v>
@@ -2350,7 +2350,7 @@
         <v>38</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H39" s="8">
         <v>16070730</v>
@@ -2364,7 +2364,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B40" s="5">
         <v>0.77700000000000002</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B41" s="5">
         <v>0.77500000000000002</v>
@@ -2428,7 +2428,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B42" s="5">
         <v>0.77300000000000002</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B43" s="5">
         <v>0.76800000000000002</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B44" s="5">
         <v>0.76800000000000002</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B45" s="5">
         <v>0.75900000000000001</v>
@@ -2556,7 +2556,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B46" s="5">
         <v>0.75800000000000001</v>
@@ -2588,7 +2588,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B47" s="5">
         <v>0.75600000000000001</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B48" s="5">
         <v>0.753</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B49" s="5">
         <v>0.753</v>
@@ -2684,7 +2684,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B50" s="5">
         <v>0.752</v>
@@ -2716,7 +2716,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B51" s="5">
         <v>0.75</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5">
         <v>0.74</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B53" s="5">
         <v>0.72799999999999998</v>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B54" s="5">
         <v>0.70499999999999996</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B55" s="5">
         <v>0.69899999999999995</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B56" s="5">
         <v>0.69499999999999995</v>
@@ -2908,7 +2908,7 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B57" s="5">
         <v>0.69299999999999995</v>
@@ -2940,7 +2940,7 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B58" s="5">
         <v>0.69199999999999995</v>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B59" s="5">
         <v>0.67</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B60" s="5">
         <v>0.66800000000000004</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B61" s="5">
         <v>0.66500000000000004</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B62" s="9">
         <v>0.66300000000000003</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B63" s="9">
         <v>0.65700000000000003</v>
@@ -3132,7 +3132,7 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B64" s="9">
         <v>0.65500000000000003</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B65" s="9">
         <v>0.64</v>
@@ -3182,7 +3182,7 @@
         <v>21</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H65" s="12">
         <v>10010900</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B66" s="9">
         <v>0.63500000000000001</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B67" s="9">
         <v>0.628</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B68" s="9">
         <v>0.626</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B69" s="9">
         <v>0.60799999999999998</v>
@@ -3324,7 +3324,7 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B70" s="9">
         <v>0.60799999999999998</v>
@@ -3356,7 +3356,7 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B71" s="9">
         <v>0.60699999999999998</v>
@@ -3374,7 +3374,7 @@
         <v>8</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H71" s="12">
         <v>5482000</v>
@@ -3388,7 +3388,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B72" s="9">
         <v>0.60099999999999998</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B73" s="9">
         <v>0.60099999999999998</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B74" s="9">
         <v>0.59699999999999998</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B75" s="9">
         <v>0.59599999999999997</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B76" s="9">
         <v>0.59</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B77" s="9">
         <v>0.59</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B78" s="9">
         <v>0.58699999999999997</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B79" s="9">
         <v>0.58599999999999997</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B80" s="9">
         <v>0.58199999999999996</v>
@@ -3676,7 +3676,7 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B81" s="9">
         <v>0.57799999999999996</v>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B82" s="9">
         <v>0.57799999999999996</v>
@@ -3740,7 +3740,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B83" s="9">
         <v>0.56999999999999995</v>
@@ -3772,7 +3772,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B84" s="9">
         <v>0.56699999999999995</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B85" s="9">
         <v>0.56399999999999995</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B86" s="9">
         <v>0.55600000000000005</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B87" s="9">
         <v>0.55500000000000005</v>
@@ -3900,7 +3900,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B88" s="9">
         <v>0.55100000000000005</v>
@@ -3932,7 +3932,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B89" s="9">
         <v>0.54900000000000004</v>
@@ -3964,7 +3964,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B90" s="9">
         <v>0.54700000000000004</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B91" s="9">
         <v>0.54500000000000004</v>
@@ -4014,7 +4014,7 @@
         <v>6</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H91" s="12">
         <v>593600</v>
@@ -4028,7 +4028,7 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B92" s="9">
         <v>0.53800000000000003</v>
@@ -4046,7 +4046,7 @@
         <v>26</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H92" s="12">
         <v>13770012</v>
@@ -4060,7 +4060,7 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B93" s="9">
         <v>0.53100000000000003</v>
@@ -4092,7 +4092,7 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B94" s="9">
         <v>0.52700000000000002</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B95" s="9">
         <v>0.52500000000000002</v>
@@ -4142,7 +4142,7 @@
         <v>3</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H95" s="12">
         <v>22000</v>
@@ -4156,7 +4156,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B96" s="9">
         <v>0.52100000000000002</v>
@@ -4174,7 +4174,7 @@
         <v>3</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H96" s="12">
         <v>27000</v>
@@ -4188,7 +4188,7 @@
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B97" s="9">
         <v>0.51800000000000002</v>
@@ -4206,7 +4206,7 @@
         <v>116</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H97" s="12">
         <v>46468505</v>
@@ -4220,7 +4220,7 @@
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B98" s="9">
         <v>0.51800000000000002</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B99" s="9">
         <v>0.51500000000000001</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B100" s="9">
         <v>0.51300000000000001</v>
@@ -4316,7 +4316,7 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B101" s="9">
         <v>0.51100000000000001</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B102" s="9">
         <v>0.51</v>
@@ -4380,7 +4380,7 @@
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B103" s="9">
         <v>0.498</v>
@@ -4412,7 +4412,7 @@
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B104" s="9">
         <v>0.496</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B105" s="9">
         <v>0.48899999999999999</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B106" s="9">
         <v>0.48899999999999999</v>
@@ -4508,7 +4508,7 @@
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B107" s="13">
         <v>0.48699999999999999</v>
@@ -4540,7 +4540,7 @@
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B108" s="13">
         <v>0.48299999999999998</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B109" s="13">
         <v>0.47799999999999998</v>
@@ -4604,7 +4604,7 @@
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B110" s="13">
         <v>0.47099999999999997</v>
@@ -4636,7 +4636,7 @@
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B111" s="13">
         <v>0.46800000000000003</v>
@@ -4668,7 +4668,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B112" s="13">
         <v>0.45700000000000002</v>
@@ -4700,7 +4700,7 @@
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B113" s="13">
         <v>0.45500000000000002</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B114" s="13">
         <v>0.45400000000000001</v>
@@ -4764,7 +4764,7 @@
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B115" s="13">
         <v>0.44</v>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B116" s="13">
         <v>0.437</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B117" s="13">
         <v>0.432</v>
@@ -4860,7 +4860,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B118" s="13">
         <v>0.42699999999999999</v>
@@ -4892,7 +4892,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B119" s="13">
         <v>0.42099999999999999</v>
@@ -4924,7 +4924,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B120" s="13">
         <v>0.40699999999999997</v>
@@ -4942,7 +4942,7 @@
         <v>3</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H120" s="16">
         <v>13340</v>
@@ -4956,7 +4956,7 @@
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B121" s="13">
         <v>0.39700000000000002</v>
@@ -4988,7 +4988,7 @@
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B122" s="13">
         <v>0.39</v>
@@ -5020,7 +5020,7 @@
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B123" s="13">
         <v>0.38600000000000001</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B124" s="13">
         <v>0.38600000000000001</v>
@@ -5084,7 +5084,7 @@
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B125" s="13">
         <v>0.38600000000000001</v>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B126" s="13">
         <v>0.35799999999999998</v>
@@ -5148,7 +5148,7 @@
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B127" s="13">
         <v>0.35399999999999998</v>
@@ -5180,7 +5180,7 @@
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B128" s="13">
         <v>0.34899999999999998</v>
@@ -5212,7 +5212,7 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B129" s="13">
         <v>0.34100000000000003</v>
@@ -5244,7 +5244,7 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B130" s="13">
         <v>0.33300000000000002</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B131" s="13">
         <v>0.33100000000000002</v>
@@ -5308,7 +5308,7 @@
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B132" s="13">
         <v>0.32800000000000001</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B133" s="13">
         <v>0.32200000000000001</v>
@@ -5372,7 +5372,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B134" s="13">
         <v>0.31900000000000001</v>
@@ -5390,7 +5390,7 @@
         <v>7</v>
       </c>
       <c r="G134" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H134" s="16">
         <v>19326030</v>
@@ -5404,7 +5404,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B135" s="13">
         <v>0.313</v>
@@ -5422,7 +5422,7 @@
         <v>3</v>
       </c>
       <c r="G135" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H135" s="16">
         <v>52800</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B136" s="13">
         <v>0.311</v>
@@ -5454,7 +5454,7 @@
         <v>2</v>
       </c>
       <c r="G136" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H136" s="16">
         <v>2080</v>
@@ -5468,7 +5468,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B137" s="13">
         <v>0.30499999999999999</v>
@@ -5486,7 +5486,7 @@
         <v>14</v>
       </c>
       <c r="G137" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H137" s="16">
         <v>644039</v>
@@ -5500,7 +5500,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B138" s="13">
         <v>0.3</v>
@@ -5532,7 +5532,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B139" s="13">
         <v>0.29099999999999998</v>
@@ -5564,7 +5564,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B140" s="13">
         <v>0.28499999999999998</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B141" s="13">
         <v>0.26700000000000002</v>
@@ -5628,7 +5628,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B142" s="13">
         <v>0.26600000000000001</v>
@@ -5660,7 +5660,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B143" s="13">
         <v>0.26</v>
@@ -5692,7 +5692,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B144" s="13">
         <v>0.26</v>
@@ -5724,7 +5724,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B145" s="13">
         <v>0.25800000000000001</v>
@@ -5756,7 +5756,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B146" s="13">
         <v>0.251</v>
@@ -5788,7 +5788,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B147" s="13">
         <v>0.25</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B148" s="13">
         <v>0.24399999999999999</v>
@@ -5838,7 +5838,7 @@
         <v>3</v>
       </c>
       <c r="G148" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H148" s="16">
         <v>7850</v>
@@ -5852,7 +5852,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B149" s="13">
         <v>0.23699999999999999</v>
@@ -5884,7 +5884,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B150" s="13">
         <v>0.23400000000000001</v>
@@ -5902,7 +5902,7 @@
         <v>2</v>
       </c>
       <c r="G150" s="14" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H150" s="16">
         <v>57830</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B151" s="13">
         <v>0.21</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="17" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B152" s="17">
         <v>0.21</v>
@@ -5980,7 +5980,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B153" s="17">
         <v>0.20899999999999999</v>
@@ -6012,7 +6012,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B154" s="17">
         <v>0.20799999999999999</v>
@@ -6030,7 +6030,7 @@
         <v>5</v>
       </c>
       <c r="G154" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H154" s="20">
         <v>14750</v>
@@ -6044,7 +6044,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B155" s="17">
         <v>0.20799999999999999</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B156" s="17">
         <v>0.17899999999999999</v>
@@ -6108,7 +6108,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B157" s="17">
         <v>0.17399999999999999</v>
@@ -6140,7 +6140,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="17" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B158" s="17">
         <v>0.17</v>
@@ -6172,7 +6172,7 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="17" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B159" s="17">
         <v>0.16800000000000001</v>
@@ -6204,7 +6204,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="17" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B160" s="17">
         <v>0.16700000000000001</v>
@@ -6222,7 +6222,7 @@
         <v>2</v>
       </c>
       <c r="G160" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H160" s="20">
         <v>21700</v>
@@ -6236,7 +6236,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="17" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B161" s="17">
         <v>0.16700000000000001</v>
@@ -6254,7 +6254,7 @@
         <v>22</v>
       </c>
       <c r="G161" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H161" s="20">
         <v>21638400</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="17" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B162" s="17">
         <v>0.161</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="17" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B163" s="17">
         <v>0.153</v>
@@ -6332,7 +6332,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B164" s="17">
         <v>0.14599999999999999</v>
@@ -6364,7 +6364,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="17" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B165" s="17">
         <v>0.14399999999999999</v>
@@ -6396,7 +6396,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="17" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B166" s="17">
         <v>0.14099999999999999</v>
@@ -6414,7 +6414,7 @@
         <v>2</v>
       </c>
       <c r="G166" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H166" s="20">
         <v>12450</v>
@@ -6428,7 +6428,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="17" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B167" s="17">
         <v>0.13900000000000001</v>
@@ -6446,7 +6446,7 @@
         <v>3</v>
       </c>
       <c r="G167" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H167" s="20">
         <v>11570</v>
@@ -6460,7 +6460,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="17" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B168" s="17">
         <v>0.13700000000000001</v>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="17" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B169" s="17">
         <v>0.13600000000000001</v>
@@ -6524,7 +6524,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B170" s="17">
         <v>0.13500000000000001</v>
@@ -6556,7 +6556,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="17" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B171" s="17">
         <v>0.13400000000000001</v>
@@ -6574,7 +6574,7 @@
         <v>5</v>
       </c>
       <c r="G171" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H171" s="20">
         <v>401420</v>
@@ -6588,7 +6588,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="17" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B172" s="17">
         <v>0.13400000000000001</v>
@@ -6620,7 +6620,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B173" s="17">
         <v>0.13400000000000001</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="17" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B174" s="17">
         <v>0.128</v>
@@ -6684,7 +6684,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="17" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B175" s="17">
         <v>0.128</v>
@@ -6716,7 +6716,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="17" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B176" s="17">
         <v>0.126</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="17" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B177" s="17">
         <v>0.125</v>
@@ -6780,7 +6780,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B178" s="17">
         <v>0.11600000000000001</v>
@@ -6812,7 +6812,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="17" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B179" s="17">
         <v>0.108</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B180" s="17">
         <v>0.108</v>
@@ -6862,7 +6862,7 @@
         <v>5</v>
       </c>
       <c r="G180" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H180" s="20">
         <v>15682</v>
@@ -6876,7 +6876,7 @@
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="17" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B181" s="17">
         <v>0.107</v>
@@ -6908,7 +6908,7 @@
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="17" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B182" s="17">
         <v>9.9000000000000005E-2</v>
@@ -6926,7 +6926,7 @@
         <v>3</v>
       </c>
       <c r="G182" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H182" s="20">
         <v>76680</v>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B183" s="17">
         <v>9.5000000000000001E-2</v>
@@ -6972,7 +6972,7 @@
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="17" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B184" s="17">
         <v>9.4E-2</v>
@@ -7004,7 +7004,7 @@
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="17" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B185" s="17">
         <v>8.3000000000000004E-2</v>
@@ -7036,7 +7036,7 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="17" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B186" s="17">
         <v>7.8E-2</v>
@@ -7068,7 +7068,7 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="17" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B187" s="17">
         <v>7.5999999999999998E-2</v>
@@ -7100,7 +7100,7 @@
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="17" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B188" s="17">
         <v>7.0999999999999994E-2</v>
@@ -7132,7 +7132,7 @@
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B189" s="17">
         <v>6.8000000000000005E-2</v>
@@ -7150,7 +7150,7 @@
         <v>11</v>
       </c>
       <c r="G189" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H189" s="20">
         <v>5595774</v>
@@ -7164,7 +7164,7 @@
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="17" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B190" s="17">
         <v>6.6000000000000003E-2</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="17" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B191" s="17">
         <v>6.6000000000000003E-2</v>
@@ -7228,7 +7228,7 @@
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="17" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B192" s="17">
         <v>6.4000000000000001E-2</v>
@@ -7246,7 +7246,7 @@
         <v>4</v>
       </c>
       <c r="G192" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H192" s="20">
         <v>92250</v>
@@ -7260,7 +7260,7 @@
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="17" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B193" s="17">
         <v>6.3E-2</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="17" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B194" s="17">
         <v>5.6000000000000001E-2</v>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B195" s="17">
         <v>5.3999999999999999E-2</v>
@@ -7356,7 +7356,7 @@
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="17" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B196" s="17">
         <v>5.3999999999999999E-2</v>
@@ -7374,7 +7374,7 @@
         <v>2</v>
       </c>
       <c r="G196" s="18" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H196" s="20">
         <v>1450</v>
@@ -7388,7 +7388,7 @@
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="21" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B197" s="21">
         <v>0.05</v>
@@ -7420,7 +7420,7 @@
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="21" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B198" s="21">
         <v>4.4999999999999998E-2</v>
@@ -7452,7 +7452,7 @@
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="21" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B199" s="21">
         <v>4.4999999999999998E-2</v>
@@ -7470,7 +7470,7 @@
         <v>5</v>
       </c>
       <c r="G199" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H199" s="24">
         <v>3838000</v>
@@ -7484,7 +7484,7 @@
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="21" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B200" s="21">
         <v>4.4999999999999998E-2</v>
@@ -7502,7 +7502,7 @@
         <v>10</v>
       </c>
       <c r="G200" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H200" s="24">
         <v>10847500</v>
@@ -7516,7 +7516,7 @@
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="21" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B201" s="21">
         <v>4.3999999999999997E-2</v>
@@ -7548,7 +7548,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="21" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B202" s="21">
         <v>4.2999999999999997E-2</v>
@@ -7580,7 +7580,7 @@
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="21" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B203" s="21">
         <v>4.2999999999999997E-2</v>
@@ -7612,7 +7612,7 @@
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="21" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B204" s="21">
         <v>4.2000000000000003E-2</v>
@@ -7644,7 +7644,7 @@
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="21" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B205" s="21">
         <v>0.04</v>
@@ -7676,7 +7676,7 @@
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="21" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B206" s="21">
         <v>3.3000000000000002E-2</v>
@@ -7708,7 +7708,7 @@
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="21" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B207" s="21">
         <v>2.7E-2</v>
@@ -7740,7 +7740,7 @@
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="21" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B208" s="21">
         <v>2.5999999999999999E-2</v>
@@ -7758,7 +7758,7 @@
         <v>2</v>
       </c>
       <c r="G208" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H208" s="24">
         <v>7670</v>
@@ -7772,7 +7772,7 @@
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="21" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B209" s="21">
         <v>2.1000000000000001E-2</v>
@@ -7804,7 +7804,7 @@
     </row>
     <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="21" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B210" s="21">
         <v>0.02</v>
@@ -7822,7 +7822,7 @@
         <v>2</v>
       </c>
       <c r="G210" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H210" s="24">
         <v>159600</v>
@@ -7836,7 +7836,7 @@
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="21" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B211" s="21">
         <v>1.7999999999999999E-2</v>
@@ -7854,7 +7854,7 @@
         <v>15</v>
       </c>
       <c r="G211" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H211" s="24">
         <v>9637050</v>
@@ -7868,7 +7868,7 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="21" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B212" s="21">
         <v>1.4999999999999999E-2</v>
@@ -7900,7 +7900,7 @@
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="21" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B213" s="21">
         <v>1.2E-2</v>
@@ -7932,7 +7932,7 @@
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="21" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B214" s="21">
         <v>1.0999999999999999E-2</v>
@@ -7964,7 +7964,7 @@
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="21" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B215" s="21">
         <v>0.01</v>
@@ -7982,7 +7982,7 @@
         <v>3</v>
       </c>
       <c r="G215" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H215" s="24">
         <v>39200</v>
@@ -7996,7 +7996,7 @@
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="21" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B216" s="21">
         <v>0.01</v>
@@ -8028,7 +8028,7 @@
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="21" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B217" s="21">
         <v>8.9999999999999993E-3</v>
@@ -8060,7 +8060,7 @@
     </row>
     <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="21" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B218" s="21">
         <v>4.0000000000000001E-3</v>
@@ -8092,7 +8092,7 @@
     </row>
     <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B219" s="21">
         <v>4.0000000000000001E-3</v>
@@ -8124,7 +8124,7 @@
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="21" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B220" s="21">
         <v>2E-3</v>
@@ -8156,7 +8156,7 @@
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="21" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="B221" s="21">
         <v>2E-3</v>
@@ -8174,7 +8174,7 @@
         <v>2</v>
       </c>
       <c r="G221" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H221" s="24">
         <v>199200</v>
@@ -8188,7 +8188,7 @@
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="21" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B222" s="21">
         <v>1E-3</v>
@@ -8220,7 +8220,7 @@
     </row>
     <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="21" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B223" s="21">
         <v>0</v>
@@ -8238,7 +8238,7 @@
         <v>3</v>
       </c>
       <c r="G223" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H223" s="24">
         <v>6960600</v>
@@ -8252,7 +8252,7 @@
     </row>
     <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="21" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B224" s="21">
         <v>0</v>
@@ -8270,7 +8270,7 @@
         <v>2</v>
       </c>
       <c r="G224" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H224" s="24">
         <v>25000</v>
@@ -8284,7 +8284,7 @@
     </row>
     <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="21" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B225" s="21">
         <v>0</v>
@@ -8302,7 +8302,7 @@
         <v>1</v>
       </c>
       <c r="G225" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H225" s="24">
         <v>3500</v>
@@ -8316,7 +8316,7 @@
     </row>
     <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="21" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B226" s="21">
         <v>0</v>
@@ -8334,7 +8334,7 @@
         <v>1</v>
       </c>
       <c r="G226" s="22" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H226" s="24">
         <v>20000000</v>

</xml_diff>